<commit_message>
increased resolution on flybys and updated Closest_Approach_Comparison_Table
</commit_message>
<xml_diff>
--- a/Closest_Approach_Comparison_Table.xlsx
+++ b/Closest_Approach_Comparison_Table.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Callisto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21EF4001-23AD-4529-9509-FC597B456CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74DD7EC-CF24-425E-B9A9-2A9DB2C06B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Juice_CA" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Orbit</t>
   </si>
@@ -180,14 +180,17 @@
       <t xml:space="preserve"> (IAU Sun)</t>
     </r>
   </si>
+  <si>
+    <t>Ionosphere Time (s)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -849,9 +852,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -902,13 +905,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
@@ -926,64 +929,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1339,21 +1345,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="12.77734375" customWidth="1"/>
-    <col min="8" max="8" width="6.21875" customWidth="1"/>
-    <col min="9" max="16" width="12.77734375" customWidth="1"/>
+    <col min="1" max="8" width="12.77734375" customWidth="1"/>
+    <col min="9" max="9" width="6.21875" customWidth="1"/>
+    <col min="10" max="17" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1375,77 +1381,83 @@
       <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="H1" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>1</v>
       </c>
       <c r="B2" s="23">
         <v>76.008556290000001</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="33">
         <v>-20.576458446815</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D2" s="34">
         <v>-173.168187890063</v>
       </c>
       <c r="E2" s="18">
         <v>-3.78737485</v>
       </c>
-      <c r="F2" s="36">
+      <c r="F2" s="34">
         <v>95.057387521084607</v>
       </c>
       <c r="G2" s="6">
         <v>103.6283007</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="16">
+        <v>0</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="23">
+      <c r="K2" s="23">
         <v>76.825901959999996</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>10.8495046901939</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>-63.1587020901922</v>
       </c>
-      <c r="M2" s="19">
+      <c r="N2" s="19">
         <v>3.158816184</v>
       </c>
-      <c r="N2" s="37">
+      <c r="O2" s="35">
         <v>-12.2416154151553</v>
       </c>
-      <c r="O2" s="14">
+      <c r="P2" s="14">
         <v>39.87997816</v>
       </c>
-      <c r="P2" s="39"/>
+      <c r="Q2" s="37"/>
     </row>
-    <row r="3" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1455,42 +1467,45 @@
       <c r="C3" s="2">
         <v>-160.91597064246301</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="35">
         <v>-74.452379038560494</v>
       </c>
       <c r="E3" s="18">
         <v>-1.4821999850000001</v>
       </c>
-      <c r="F3" s="37">
+      <c r="F3" s="35">
         <v>-81.424176087898104</v>
       </c>
       <c r="G3" s="6">
         <v>144.82807750000001</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="H3" s="15">
+        <v>0</v>
+      </c>
+      <c r="J3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="22">
+      <c r="K3" s="22">
         <v>87.973532910000003</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>-170.345076975626</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>-97.036359546940105</v>
       </c>
-      <c r="M3" s="18">
+      <c r="N3" s="18">
         <v>-3.4607276489999999</v>
       </c>
-      <c r="N3" s="37">
+      <c r="O3" s="35">
         <v>-57.316449625484303</v>
       </c>
-      <c r="O3" s="6">
+      <c r="P3" s="6">
         <v>176.88572790000001</v>
       </c>
-      <c r="P3" s="40"/>
+      <c r="Q3" s="38"/>
     </row>
-    <row r="4" spans="1:16" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1500,89 +1515,95 @@
       <c r="C4" s="4">
         <v>-165.59210418246801</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="36">
         <v>-75.998071750742795</v>
       </c>
       <c r="E4" s="20">
         <v>-2.7551602700000002</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="36">
         <v>43.3571173862099</v>
       </c>
       <c r="G4" s="7">
         <v>151.74531959999999</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="H4" s="15">
+        <v>0</v>
+      </c>
+      <c r="J4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="24">
+      <c r="K4" s="24">
         <v>85.465527929999993</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
         <v>10.0928461188117</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>-104.500342606548</v>
       </c>
-      <c r="M4" s="20">
+      <c r="N4" s="20">
         <v>-3.1069623960000001</v>
       </c>
-      <c r="N4" s="38">
+      <c r="O4" s="36">
         <v>-153.50030892427401</v>
       </c>
-      <c r="O4" s="7">
+      <c r="P4" s="7">
         <v>6.24716498</v>
       </c>
-      <c r="P4" s="41"/>
+      <c r="Q4" s="39"/>
     </row>
-    <row r="5" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>4</v>
       </c>
       <c r="B5" s="23">
         <v>129.89413289999999</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="33">
         <v>-18.5777603401616</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="34">
         <v>144.01995169624001</v>
       </c>
       <c r="E5" s="19">
         <v>-3.8935851380000002</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="34">
         <v>21.996121772671401</v>
       </c>
       <c r="G5" s="14">
         <v>128.12727570000001</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="H5" s="16">
+        <v>110</v>
+      </c>
+      <c r="J5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="23">
+      <c r="K5" s="23">
         <v>90.799102250000004</v>
       </c>
-      <c r="K5" s="35">
+      <c r="L5" s="33">
         <v>12.485467490857101</v>
       </c>
-      <c r="L5" s="42">
+      <c r="M5" s="40">
         <v>-153.903696861653</v>
       </c>
-      <c r="M5" s="19">
+      <c r="N5" s="19">
         <v>-1.8859858940000001</v>
       </c>
-      <c r="N5" s="36">
+      <c r="O5" s="34">
         <v>27.246025075013801</v>
       </c>
-      <c r="O5" s="14">
+      <c r="P5" s="14">
         <v>51.548688550000001</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="Q5" s="45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -1592,42 +1613,45 @@
       <c r="C6" s="2">
         <v>-78.699217260267403</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="35">
         <v>142.60883593958201</v>
       </c>
       <c r="E6" s="18">
         <v>1.3771442540000001</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="35">
         <v>146.689073258364</v>
       </c>
       <c r="G6" s="6">
         <v>97.452151450000002</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="H6" s="15">
+        <v>450</v>
+      </c>
+      <c r="J6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="22">
+      <c r="K6" s="22">
         <v>92.351720119999996</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>-18.248924218414398</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>91.964543732483904</v>
       </c>
-      <c r="M6" s="18">
+      <c r="N6" s="18">
         <v>-4.2507527759999997</v>
       </c>
-      <c r="N6" s="37">
+      <c r="O6" s="35">
         <v>112.640068729061</v>
       </c>
-      <c r="O6" s="6">
+      <c r="P6" s="6">
         <v>163.8755214</v>
       </c>
-      <c r="P6" s="26"/>
+      <c r="Q6" s="46"/>
     </row>
-    <row r="7" spans="1:16" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1637,42 +1661,45 @@
       <c r="C7" s="2">
         <v>-85.069149638486095</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="35">
         <v>141.126765366379</v>
       </c>
       <c r="E7" s="18">
         <v>2.7316141740000002</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="35">
         <v>-88.565378422761398</v>
       </c>
       <c r="G7" s="6">
         <v>106.6805488</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="H7" s="15">
+        <v>450</v>
+      </c>
+      <c r="J7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="24">
+      <c r="K7" s="24">
         <v>90</v>
       </c>
-      <c r="K7" s="4">
+      <c r="L7" s="4">
         <v>-19.064547431332201</v>
       </c>
-      <c r="L7" s="3">
+      <c r="M7" s="3">
         <v>88.783171417706797</v>
       </c>
-      <c r="M7" s="20">
+      <c r="N7" s="20">
         <v>1.0016548000000001</v>
       </c>
-      <c r="N7" s="38">
+      <c r="O7" s="36">
         <v>2.3324190003984002</v>
       </c>
-      <c r="O7" s="7">
+      <c r="P7" s="7">
         <v>159.68221159999999</v>
       </c>
-      <c r="P7" s="27"/>
+      <c r="Q7" s="47"/>
     </row>
-    <row r="8" spans="1:16" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1682,42 +1709,45 @@
       <c r="C8" s="2">
         <v>-88.598901898441198</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="35">
         <v>139.583635595342</v>
       </c>
       <c r="E8" s="18">
         <v>-4.2280143560000001</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="35">
         <v>36.222927524571901</v>
       </c>
       <c r="G8" s="6">
         <v>115.4440261</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="H8" s="15">
+        <v>175</v>
+      </c>
+      <c r="J8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="32">
+      <c r="K8" s="30">
         <v>76.403189679999997</v>
       </c>
-      <c r="K8" s="43">
+      <c r="L8" s="41">
         <v>-15.064835068844101</v>
       </c>
-      <c r="L8" s="44">
+      <c r="M8" s="42">
         <v>17.358876802217999</v>
       </c>
-      <c r="M8" s="33">
+      <c r="N8" s="31">
         <v>-2.413465967</v>
       </c>
-      <c r="N8" s="45">
+      <c r="O8" s="43">
         <v>-50.858067208705101</v>
       </c>
-      <c r="O8" s="34">
+      <c r="P8" s="32">
         <v>91.641126779999993</v>
       </c>
-      <c r="P8" s="46"/>
+      <c r="Q8" s="44"/>
     </row>
-    <row r="9" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1727,20 +1757,23 @@
       <c r="C9" s="2">
         <v>-88.540274305872103</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="35">
         <v>137.99949809499401</v>
       </c>
       <c r="E9" s="18">
         <v>2.3259396309999998</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="35">
         <v>161.03437765107299</v>
       </c>
       <c r="G9" s="6">
         <v>122.3029186</v>
       </c>
+      <c r="H9" s="15">
+        <v>100</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -1750,46 +1783,52 @@
       <c r="C10" s="4">
         <v>-38.714200410945097</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="36">
         <v>136.375188300942</v>
       </c>
       <c r="E10" s="20">
         <v>2.1984256750000002</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="36">
         <v>-74.121245207587506</v>
       </c>
       <c r="G10" s="7">
         <v>168.69653479999999</v>
       </c>
-      <c r="K10" s="28"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="29"/>
+      <c r="H10" s="15">
+        <v>0</v>
+      </c>
+      <c r="L10" s="26"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="27"/>
     </row>
-    <row r="11" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>10</v>
       </c>
       <c r="B11" s="23">
         <v>99.827328699999995</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="33">
         <v>157.791319370661</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D11" s="34">
         <v>128.96401988182001</v>
       </c>
       <c r="E11" s="19">
         <v>4.1706659620000002</v>
       </c>
-      <c r="F11" s="36">
+      <c r="F11" s="34">
         <v>-170.35641565085601</v>
       </c>
       <c r="G11" s="14">
         <v>19.44942331</v>
       </c>
+      <c r="H11" s="16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -1799,20 +1838,23 @@
       <c r="C12" s="2">
         <v>148.97101253802401</v>
       </c>
-      <c r="D12" s="37">
+      <c r="D12" s="35">
         <v>127.36482403358001</v>
       </c>
       <c r="E12" s="18">
         <v>-0.72448691899999995</v>
       </c>
-      <c r="F12" s="37">
+      <c r="F12" s="35">
         <v>-45.520873880956501</v>
       </c>
       <c r="G12" s="6">
         <v>8.6137101559999998</v>
       </c>
+      <c r="H12" s="15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:16" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -1822,43 +1864,49 @@
       <c r="C13" s="4">
         <v>71.7405413475486</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="36">
         <v>-58.230419616551899</v>
       </c>
       <c r="E13" s="20">
         <v>1.334758586</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="36">
         <v>-147.56779179471999</v>
       </c>
       <c r="G13" s="7">
         <v>101.522659</v>
       </c>
+      <c r="H13" s="17">
+        <v>350</v>
+      </c>
     </row>
-    <row r="14" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>13</v>
       </c>
       <c r="B14" s="23">
         <v>51.508677820000003</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="33">
         <v>61.807764176066598</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="34">
         <v>119.492629235343</v>
       </c>
       <c r="E14" s="19">
         <v>4.4746277020000003</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F14" s="34">
         <v>-141.41275429345299</v>
       </c>
       <c r="G14" s="14">
         <v>88.592421459999997</v>
       </c>
+      <c r="H14" s="15">
+        <v>450</v>
+      </c>
     </row>
-    <row r="15" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -1868,20 +1916,23 @@
       <c r="C15" s="2">
         <v>88.768090896494598</v>
       </c>
-      <c r="D15" s="37">
+      <c r="D15" s="35">
         <v>117.878271675251</v>
       </c>
       <c r="E15" s="18">
         <v>-2.4462538</v>
       </c>
-      <c r="F15" s="37">
+      <c r="F15" s="35">
         <v>-16.558494316550799</v>
       </c>
       <c r="G15" s="6">
         <v>70.524759689999996</v>
       </c>
+      <c r="H15" s="15">
+        <v>450</v>
+      </c>
     </row>
-    <row r="16" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -1891,20 +1942,23 @@
       <c r="C16" s="2">
         <v>87.672285950219901</v>
       </c>
-      <c r="D16" s="37">
+      <c r="D16" s="35">
         <v>116.244213380948</v>
       </c>
       <c r="E16" s="18">
         <v>-1.46958126</v>
       </c>
-      <c r="F16" s="37">
+      <c r="F16" s="35">
         <v>108.308460606834</v>
       </c>
       <c r="G16" s="6">
         <v>75.491922759999994</v>
       </c>
+      <c r="H16" s="15">
+        <v>450</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -1914,20 +1968,23 @@
       <c r="C17" s="2">
         <v>90.258303690275199</v>
       </c>
-      <c r="D17" s="37">
+      <c r="D17" s="35">
         <v>114.61640181145501</v>
       </c>
       <c r="E17" s="18">
         <v>4.3940168350000004</v>
       </c>
-      <c r="F17" s="37">
+      <c r="F17" s="35">
         <v>-126.83158913395999</v>
       </c>
       <c r="G17" s="6">
         <v>80.840828549999998</v>
       </c>
+      <c r="H17" s="15">
+        <v>450</v>
+      </c>
     </row>
-    <row r="18" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -1937,20 +1994,23 @@
       <c r="C18" s="4">
         <v>154.49981661960101</v>
       </c>
-      <c r="D18" s="38">
+      <c r="D18" s="36">
         <v>113.067145516587</v>
       </c>
       <c r="E18" s="20">
         <v>-3.084926077</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F18" s="36">
         <v>-2.01784065989174</v>
       </c>
       <c r="G18" s="7">
         <v>48.15514787</v>
       </c>
+      <c r="H18" s="17">
+        <v>450</v>
+      </c>
     </row>
-    <row r="19" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -1960,20 +2020,23 @@
       <c r="C19" s="2">
         <v>170.41425567297401</v>
       </c>
-      <c r="D19" s="37">
+      <c r="D19" s="35">
         <v>105.656737035996</v>
       </c>
       <c r="E19" s="18">
         <v>2.1439229759999998</v>
       </c>
-      <c r="F19" s="37">
+      <c r="F19" s="35">
         <v>-98.165552947404706</v>
       </c>
       <c r="G19" s="6">
         <v>48.733771240000003</v>
       </c>
+      <c r="H19" s="15">
+        <v>350</v>
+      </c>
     </row>
-    <row r="20" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
         <v>19</v>
       </c>
@@ -1983,20 +2046,23 @@
       <c r="C20" s="2">
         <v>-158.28671435084499</v>
       </c>
-      <c r="D20" s="37">
+      <c r="D20" s="35">
         <v>-157.20105953491699</v>
       </c>
       <c r="E20" s="18">
         <v>3.3948574640000002</v>
       </c>
-      <c r="F20" s="37">
+      <c r="F20" s="35">
         <v>-138.65340878056401</v>
       </c>
       <c r="G20" s="6">
         <v>134.39394809999999</v>
       </c>
+      <c r="H20" s="15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>20</v>
       </c>
@@ -2006,20 +2072,23 @@
       <c r="C21" s="2">
         <v>-16.6761656951888</v>
       </c>
-      <c r="D21" s="37">
+      <c r="D21" s="35">
         <v>33.637267614280098</v>
       </c>
       <c r="E21" s="18">
         <v>4.2923113490000002</v>
       </c>
-      <c r="F21" s="37">
+      <c r="F21" s="35">
         <v>-128.714945956186</v>
       </c>
       <c r="G21" s="6">
         <v>106.78706990000001</v>
       </c>
+      <c r="H21" s="15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>21</v>
       </c>
@@ -2029,25 +2098,28 @@
       <c r="C22" s="4">
         <v>96.342378069501905</v>
       </c>
-      <c r="D22" s="38">
+      <c r="D22" s="36">
         <v>97.5850977810735</v>
       </c>
       <c r="E22" s="20">
         <v>-3.1790829309999999</v>
       </c>
-      <c r="F22" s="38">
+      <c r="F22" s="36">
         <v>-159.63424203762699</v>
       </c>
       <c r="G22" s="7">
         <v>76.031399629999996</v>
+      </c>
+      <c r="H22" s="17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="P5:P7"/>
+    <mergeCell ref="Q5:Q7"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B22">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -2059,6 +2131,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C22">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="num" val="-180"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="180"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="num" val="-180"/>
@@ -2070,20 +2154,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D22">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="num" val="-180"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="num" val="180"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E2:E22">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="-4.5"/>
         <cfvo type="percentile" val="50"/>
@@ -2095,7 +2167,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F22">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="num" val="-180"/>
         <cfvo type="percentile" val="50"/>
@@ -2107,6 +2179,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G22">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="180"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K8">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2118,10 +2202,10 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="L2:L8 L10">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="-180"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="num" val="180"/>
         <color rgb="FFF8696B"/>
@@ -2130,7 +2214,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K8 K10">
+  <conditionalFormatting sqref="M2:M8">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="-180"/>
@@ -2142,8 +2226,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L8">
+  <conditionalFormatting sqref="N2:N8">
     <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="-4.5"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="4.5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O8">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="-180"/>
         <cfvo type="percentile" val="50"/>
@@ -2154,32 +2250,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M8">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="num" val="-4.5"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="num" val="4.5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N8">
+  <conditionalFormatting sqref="P2:P8">
     <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="-180"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="num" val="180"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O8">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -2190,6 +2262,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H22">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="25"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>